<commit_message>
Ajuste na organização da A_estrela Haversiano e teste de 10 nós
</commit_message>
<xml_diff>
--- a/Algoritmo_Rota/Planilhas/A_Estrela_Haversiano/PLN_13_10.xlsx
+++ b/Algoritmo_Rota/Planilhas/A_Estrela_Haversiano/PLN_13_10.xlsx
@@ -462,7 +462,7 @@
         <v>1223</v>
       </c>
       <c r="E2" t="n">
-        <v>0.02807377179463704</v>
+        <v>0.02826855977376302</v>
       </c>
     </row>
     <row r="3">
@@ -479,7 +479,7 @@
         <v>1272</v>
       </c>
       <c r="E3" t="n">
-        <v>0.02813696066538493</v>
+        <v>0.0281636635462443</v>
       </c>
     </row>
     <row r="4">
@@ -496,7 +496,7 @@
         <v>1224</v>
       </c>
       <c r="E4" t="n">
-        <v>0.03059898217519124</v>
+        <v>0.03076435724894206</v>
       </c>
     </row>
     <row r="5">
@@ -513,7 +513,7 @@
         <v>1272</v>
       </c>
       <c r="E5" t="n">
-        <v>0.02815361817677816</v>
+        <v>0.02792839209238688</v>
       </c>
     </row>
     <row r="6">
@@ -530,7 +530,7 @@
         <v>1221</v>
       </c>
       <c r="E6" t="n">
-        <v>0.0281095822652181</v>
+        <v>0.0280669371287028</v>
       </c>
     </row>
     <row r="7">
@@ -547,7 +547,7 @@
         <v>1068</v>
       </c>
       <c r="E7" t="n">
-        <v>0.02815911769866943</v>
+        <v>0.02815721829732259</v>
       </c>
     </row>
     <row r="8">
@@ -564,7 +564,7 @@
         <v>1057</v>
       </c>
       <c r="E8" t="n">
-        <v>0.02835159301757812</v>
+        <v>0.02821250756581624</v>
       </c>
     </row>
     <row r="9">
@@ -581,7 +581,7 @@
         <v>1068</v>
       </c>
       <c r="E9" t="n">
-        <v>0.02830394903818766</v>
+        <v>0.02816736698150635</v>
       </c>
     </row>
     <row r="10">
@@ -598,7 +598,7 @@
         <v>1221</v>
       </c>
       <c r="E10" t="n">
-        <v>0.02834920088450114</v>
+        <v>0.02811907132466634</v>
       </c>
     </row>
     <row r="11">
@@ -615,7 +615,7 @@
         <v>1057</v>
       </c>
       <c r="E11" t="n">
-        <v>0.02836179733276367</v>
+        <v>0.02914378643035889</v>
       </c>
     </row>
   </sheetData>

</xml_diff>